<commit_message>
maj bom base roulante + bille en metal
</commit_message>
<xml_diff>
--- a/Mecanique/BOM Mecanique.xlsx
+++ b/Mecanique/BOM Mecanique.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git folder\my_robot\Mecanique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33705920-C644-4187-BB4F-905671A400F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63854E0F-8258-46F5-8E25-7EA1451D72C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,8 +34,107 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={A453A135-6489-4ECD-A598-66CCDDF76889}</author>
+    <author>tc={EDD0E532-7FB4-42F8-ACF4-E41B5A9F00C8}</author>
+    <author>tc={1E753FFD-2227-47C3-B823-0491CFB53051}</author>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{A453A135-6489-4ECD-A598-66CCDDF76889}">
+      <text>
+        <t>[Commentaire à thread]
+Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
+Commentaire :
+    Les bipolaires simples sont moins chers.</t>
+      </text>
+    </comment>
+    <comment ref="B8" authorId="1" shapeId="0" xr:uid="{EDD0E532-7FB4-42F8-ACF4-E41B5A9F00C8}">
+      <text>
+        <t>[Commentaire à thread]
+Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
+Commentaire :
+    En prendre à Ares</t>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="2" shapeId="0" xr:uid="{1E753FFD-2227-47C3-B823-0491CFB53051}">
+      <text>
+        <t>[Commentaire à thread]
+Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
+Commentaire :
+    Demander au technicien</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={AB1CD8FB-3944-4F58-9773-F124CA02C732}</author>
+    <author>tc={D308E42D-385C-4779-9D12-9FEF1E79EE69}</author>
+    <author>tc={68A22E18-7B98-4346-B886-FF96C09DCDCC}</author>
+    <author>tc={0323C182-F2A4-4590-B95E-32B6190FCB2D}</author>
+    <author>tc={A0E95CFD-C201-4571-9DB1-A8E4D9268DA7}</author>
+    <author>tc={2E5A2AC7-438A-46E2-9233-5790A980370A}</author>
+  </authors>
+  <commentList>
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{AB1CD8FB-3944-4F58-9773-F124CA02C732}">
+      <text>
+        <t>[Commentaire à thread]
+Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
+Commentaire :
+    En prendre à Ares (si même dimension)</t>
+      </text>
+    </comment>
+    <comment ref="B5" authorId="1" shapeId="0" xr:uid="{D308E42D-385C-4779-9D12-9FEF1E79EE69}">
+      <text>
+        <t>[Commentaire à thread]
+Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
+Commentaire :
+    En prendre à Ares</t>
+      </text>
+    </comment>
+    <comment ref="B6" authorId="2" shapeId="0" xr:uid="{68A22E18-7B98-4346-B886-FF96C09DCDCC}">
+      <text>
+        <t>[Commentaire à thread]
+Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
+Commentaire :
+    En prendre à Ares</t>
+      </text>
+    </comment>
+    <comment ref="B7" authorId="3" shapeId="0" xr:uid="{0323C182-F2A4-4590-B95E-32B6190FCB2D}">
+      <text>
+        <t>[Commentaire à thread]
+Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
+Commentaire :
+    En prendre à Ares</t>
+      </text>
+    </comment>
+    <comment ref="B8" authorId="4" shapeId="0" xr:uid="{A0E95CFD-C201-4571-9DB1-A8E4D9268DA7}">
+      <text>
+        <t>[Commentaire à thread]
+Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
+Commentaire :
+    En prendre à Ares</t>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="5" shapeId="0" xr:uid="{2E5A2AC7-438A-46E2-9233-5790A980370A}">
+      <text>
+        <t>[Commentaire à thread]
+Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
+Commentaire :
+    En prendre à Ares</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="55">
   <si>
     <t>Mecanique/Base roulante</t>
   </si>
@@ -134,16 +233,83 @@
   </si>
   <si>
     <t>42,30mm</t>
+  </si>
+  <si>
+    <t>LPD3806-600BM-G5-24C</t>
+  </si>
+  <si>
+    <t>AliExpress</t>
+  </si>
+  <si>
+    <t>nc</t>
+  </si>
+  <si>
+    <t>Codeur : LPD3806-600BM-G5-24C</t>
+  </si>
+  <si>
+    <t>Moyeu pour axe de 5mm</t>
+  </si>
+  <si>
+    <t>GoTronic</t>
+  </si>
+  <si>
+    <t>Roulement à bille 19/6/6mm</t>
+  </si>
+  <si>
+    <t>Profilé MakerBeam 40mm</t>
+  </si>
+  <si>
+    <t>MakerBeam</t>
+  </si>
+  <si>
+    <t>Joint torique</t>
+  </si>
+  <si>
+    <t>Roue motrice</t>
+  </si>
+  <si>
+    <t>38,5mm</t>
+  </si>
+  <si>
+    <t>20mm</t>
+  </si>
+  <si>
+    <t>PLA</t>
+  </si>
+  <si>
+    <t>Impression 3D</t>
+  </si>
+  <si>
+    <t>Pivot codeur</t>
+  </si>
+  <si>
+    <t>Pivot codeur support 1</t>
+  </si>
+  <si>
+    <t>Pivot codeur support 2</t>
+  </si>
+  <si>
+    <t>Rondelle en plastique</t>
+  </si>
+  <si>
+    <t>Support batterie</t>
+  </si>
+  <si>
+    <t>Roue libre 3/4'' en métal</t>
+  </si>
+  <si>
+    <t>Support bille (roue libre 3/4'' en métal)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,6 +348,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -229,7 +401,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -252,18 +424,34 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -282,6 +470,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Arnaud CHOBERT" id="{C70F27C7-08E0-4567-A0C3-CF8061227EA5}" userId="171bb5531915668a" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -545,21 +739,63 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B2" dT="2021-07-24T13:28:44.56" personId="{C70F27C7-08E0-4567-A0C3-CF8061227EA5}" id="{A453A135-6489-4ECD-A598-66CCDDF76889}">
+    <text>Les bipolaires simples sont moins chers.</text>
+  </threadedComment>
+  <threadedComment ref="B8" dT="2021-07-24T13:48:48.54" personId="{C70F27C7-08E0-4567-A0C3-CF8061227EA5}" id="{EDD0E532-7FB4-42F8-ACF4-E41B5A9F00C8}">
+    <text>En prendre à Ares</text>
+  </threadedComment>
+  <threadedComment ref="B9" dT="2021-07-24T13:58:08.18" personId="{C70F27C7-08E0-4567-A0C3-CF8061227EA5}" id="{1E753FFD-2227-47C3-B823-0491CFB53051}">
+    <text>Demander au technicien</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="B3" dT="2021-07-24T13:49:22.73" personId="{C70F27C7-08E0-4567-A0C3-CF8061227EA5}" id="{AB1CD8FB-3944-4F58-9773-F124CA02C732}">
+    <text>En prendre à Ares (si même dimension)</text>
+  </threadedComment>
+  <threadedComment ref="B5" dT="2021-07-24T13:53:40.35" personId="{C70F27C7-08E0-4567-A0C3-CF8061227EA5}" id="{D308E42D-385C-4779-9D12-9FEF1E79EE69}">
+    <text>En prendre à Ares</text>
+  </threadedComment>
+  <threadedComment ref="B6" dT="2021-07-24T13:56:08.32" personId="{C70F27C7-08E0-4567-A0C3-CF8061227EA5}" id="{68A22E18-7B98-4346-B886-FF96C09DCDCC}">
+    <text>En prendre à Ares</text>
+  </threadedComment>
+  <threadedComment ref="B7" dT="2021-07-24T13:56:25.67" personId="{C70F27C7-08E0-4567-A0C3-CF8061227EA5}" id="{0323C182-F2A4-4590-B95E-32B6190FCB2D}">
+    <text>En prendre à Ares</text>
+  </threadedComment>
+  <threadedComment ref="B8" dT="2021-07-24T13:56:25.67" personId="{C70F27C7-08E0-4567-A0C3-CF8061227EA5}" id="{A0E95CFD-C201-4571-9DB1-A8E4D9268DA7}">
+    <text>En prendre à Ares</text>
+  </threadedComment>
+  <threadedComment ref="B9" dT="2021-07-24T13:59:06.65" personId="{C70F27C7-08E0-4567-A0C3-CF8061227EA5}" id="{2E5A2AC7-438A-46E2-9233-5790A980370A}">
+    <text>En prendre à Ares</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.7109375" customWidth="1"/>
     <col min="2" max="2" width="55.7109375" customWidth="1"/>
-    <col min="3" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" style="11" customWidth="1"/>
-    <col min="7" max="10" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.85546875" style="15" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" style="15" customWidth="1"/>
     <col min="11" max="11" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -579,7 +815,7 @@
       <c r="E1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="10" t="s">
         <v>19</v>
       </c>
       <c r="G1" s="7" t="s">
@@ -615,7 +851,7 @@
         <f>C2*D2</f>
         <v>41.8</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="9">
         <v>2</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -624,29 +860,205 @@
       <c r="I2" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="8" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="3">
+        <v>17.13</v>
+      </c>
+      <c r="D3" s="12">
+        <v>2</v>
+      </c>
+      <c r="E3" s="13">
+        <f>C3*D3</f>
+        <v>34.26</v>
+      </c>
+      <c r="F3" s="11">
+        <v>0</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="3">
+        <f>7.9 / 2</f>
+        <v>3.95</v>
+      </c>
+      <c r="D4" s="1">
+        <v>4</v>
+      </c>
+      <c r="E4" s="3">
+        <f>C4*D4</f>
+        <v>15.8</v>
+      </c>
+      <c r="F4" s="11">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="14">
+        <v>32850</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5" s="3">
+        <f>C5*D5</f>
+        <v>6.4</v>
+      </c>
+      <c r="F5" s="11">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" s="14">
+        <v>32866</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
+      <c r="E6" s="16">
+        <f>C6*D6</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F6" s="11">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="14">
+        <v>24760</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="F7" s="11">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="14">
+        <v>100056</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" s="14">
+        <v>100056</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2</v>
+      </c>
+      <c r="F8" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="11">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="J2" r:id="rId1" xr:uid="{EF803173-6234-4D21-B2A0-29DFFED6055A}"/>
     <hyperlink ref="K2" r:id="rId2" xr:uid="{1FD15487-DBA8-48D0-B21A-CD82C5F0DDA1}"/>
+    <hyperlink ref="J3" r:id="rId3" display="Lien" xr:uid="{590ADCCA-8CE7-40AA-8C96-4A2D1FC3681E}"/>
+    <hyperlink ref="J4" r:id="rId4" display="https://www.gotronic.fr/art-paire-de-moyeux-alu-1998-21781.htm" xr:uid="{244CC552-A9F4-455C-BE90-80AABB27A3FC}"/>
+    <hyperlink ref="J5" r:id="rId5" display="https://www.gotronic.fr/art-roue-libre-3-4-955-21789.htm" xr:uid="{9FA631D8-4924-422F-9436-0F4CC6AD4E31}"/>
+    <hyperlink ref="J6" r:id="rId6" location="complte_desc" display="https://www.gotronic.fr/art-roulement-19-6-6mm-157.htm - complte_desc" xr:uid="{668C1373-B577-40D7-AE22-CEC46B56C596}"/>
+    <hyperlink ref="H7" r:id="rId7" display="https://www.makerbeam.com/makerbeam-40mm-8p-black-makerbeam.html" xr:uid="{29B79743-9F8C-4F0D-B3CD-51472A8B11E8}"/>
+    <hyperlink ref="J7" r:id="rId8" display="https://www.makerbeam.com/makerbeam-40mm-8p-black-makerbeam.html" xr:uid="{82784541-8BB1-4123-8126-54CF8432B427}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId9"/>
+  <legacyDrawing r:id="rId10"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9B52879-989E-4911-9FCB-E5FD6170BF14}">
-  <dimension ref="A1:J4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9B52879-989E-4911-9FCB-E5FD6170BF14}">
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,7 +1084,7 @@
       <c r="D1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="10" t="s">
         <v>19</v>
       </c>
       <c r="F1" s="6" t="s">
@@ -704,7 +1116,7 @@
       <c r="D2" s="1">
         <v>1</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="11">
         <v>0</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -730,7 +1142,7 @@
       <c r="D3" s="1">
         <v>2</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="11">
         <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -762,7 +1174,7 @@
       <c r="D4" s="1">
         <v>2</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="11">
         <v>0</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -781,8 +1193,166 @@
         <v>26</v>
       </c>
     </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5" s="11">
+        <v>0</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="17"/>
+      <c r="H5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2</v>
+      </c>
+      <c r="E6" s="11">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2</v>
+      </c>
+      <c r="E7" s="11">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="1">
+        <v>4</v>
+      </c>
+      <c r="E8" s="11">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2</v>
+      </c>
+      <c r="E9" s="11">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2</v>
+      </c>
+      <c r="E10" s="11">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F5:G5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
etages + maj bom
</commit_message>
<xml_diff>
--- a/Mecanique/BOM Mecanique.xlsx
+++ b/Mecanique/BOM Mecanique.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git folder\my_robot\Mecanique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63854E0F-8258-46F5-8E25-7EA1451D72C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B76E5CB-4A89-49FA-9AA8-8F58C851114A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Articles achetés" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
     <author>tc={1E753FFD-2227-47C3-B823-0491CFB53051}</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{A453A135-6489-4ECD-A598-66CCDDF76889}">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{A453A135-6489-4ECD-A598-66CCDDF76889}">
       <text>
         <t>[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
@@ -50,7 +50,7 @@
     Les bipolaires simples sont moins chers.</t>
       </text>
     </comment>
-    <comment ref="B8" authorId="1" shapeId="0" xr:uid="{EDD0E532-7FB4-42F8-ACF4-E41B5A9F00C8}">
+    <comment ref="A9" authorId="1" shapeId="0" xr:uid="{EDD0E532-7FB4-42F8-ACF4-E41B5A9F00C8}">
       <text>
         <t>[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
@@ -58,7 +58,7 @@
     En prendre à Ares</t>
       </text>
     </comment>
-    <comment ref="B9" authorId="2" shapeId="0" xr:uid="{1E753FFD-2227-47C3-B823-0491CFB53051}">
+    <comment ref="A10" authorId="2" shapeId="0" xr:uid="{1E753FFD-2227-47C3-B823-0491CFB53051}">
       <text>
         <t>[Commentaire à thread]
 Votre version d’Excel vous permet de lire ce commentaire à thread. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
@@ -134,7 +134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="64">
   <si>
     <t>Mecanique/Base roulante</t>
   </si>
@@ -299,6 +299,35 @@
   </si>
   <si>
     <t>Support bille (roue libre 3/4'' en métal)</t>
+  </si>
+  <si>
+    <t>Équerre MakerBeam L-90°</t>
+  </si>
+  <si>
+    <t>Profilé MakerBeam 300mm</t>
+  </si>
+  <si>
+    <t>Profilé MakerBeam 150mm</t>
+  </si>
+  <si>
+    <t>Groupe(s)</t>
+  </si>
+  <si>
+    <t>Base roulante</t>
+  </si>
+  <si>
+    <t>Structure</t>
+  </si>
+  <si>
+    <t>Base roulante
+Structure</t>
+  </si>
+  <si>
+    <t>Pneu (à partir d'une chambre à air de vélo)</t>
+  </si>
+  <si>
+    <t>Structure
+Etage actionneurs</t>
   </si>
 </sst>
 </file>
@@ -309,7 +338,7 @@
     <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -348,12 +377,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -401,7 +424,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -453,6 +476,49 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -741,13 +807,13 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="B2" dT="2021-07-24T13:28:44.56" personId="{C70F27C7-08E0-4567-A0C3-CF8061227EA5}" id="{A453A135-6489-4ECD-A598-66CCDDF76889}">
+  <threadedComment ref="A4" dT="2021-07-24T13:28:44.56" personId="{C70F27C7-08E0-4567-A0C3-CF8061227EA5}" id="{A453A135-6489-4ECD-A598-66CCDDF76889}">
     <text>Les bipolaires simples sont moins chers.</text>
   </threadedComment>
-  <threadedComment ref="B8" dT="2021-07-24T13:48:48.54" personId="{C70F27C7-08E0-4567-A0C3-CF8061227EA5}" id="{EDD0E532-7FB4-42F8-ACF4-E41B5A9F00C8}">
+  <threadedComment ref="A9" dT="2021-07-24T13:48:48.54" personId="{C70F27C7-08E0-4567-A0C3-CF8061227EA5}" id="{EDD0E532-7FB4-42F8-ACF4-E41B5A9F00C8}">
     <text>En prendre à Ares</text>
   </threadedComment>
-  <threadedComment ref="B9" dT="2021-07-24T13:58:08.18" personId="{C70F27C7-08E0-4567-A0C3-CF8061227EA5}" id="{1E753FFD-2227-47C3-B823-0491CFB53051}">
+  <threadedComment ref="A10" dT="2021-07-24T13:58:08.18" personId="{C70F27C7-08E0-4567-A0C3-CF8061227EA5}" id="{1E753FFD-2227-47C3-B823-0491CFB53051}">
     <text>Demander au technicien</text>
   </threadedComment>
 </ThreadedComments>
@@ -778,33 +844,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" customWidth="1"/>
-    <col min="2" max="2" width="55.7109375" customWidth="1"/>
+    <col min="1" max="1" width="55.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="17" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" style="17" customWidth="1"/>
     <col min="8" max="8" width="21.85546875" style="15" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" style="17" customWidth="1"/>
     <col min="10" max="10" width="20.7109375" style="15" customWidth="1"/>
     <col min="11" max="11" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="5" t="s">
+      <c r="A1" s="5" t="s">
         <v>2</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>5</v>
@@ -834,222 +900,359 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="3">
-        <v>20.9</v>
-      </c>
-      <c r="D2" s="1">
-        <v>2</v>
-      </c>
-      <c r="E2" s="3">
-        <f>C2*D2</f>
-        <v>41.8</v>
-      </c>
-      <c r="F2" s="9">
-        <v>2</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="3">
-        <v>17.13</v>
-      </c>
-      <c r="D3" s="12">
-        <v>2</v>
-      </c>
-      <c r="E3" s="13">
-        <f>C3*D3</f>
-        <v>34.26</v>
-      </c>
-      <c r="F3" s="11">
-        <v>0</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="I3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" s="14" t="s">
-        <v>35</v>
-      </c>
+    <row r="2" spans="1:11" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+    </row>
+    <row r="3" spans="1:11" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="3">
+        <v>20.9</v>
+      </c>
+      <c r="D4" s="17">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3">
+        <f>C4*D4</f>
+        <v>41.8</v>
+      </c>
+      <c r="F4" s="9">
+        <v>2</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="3">
+        <v>17.13</v>
+      </c>
+      <c r="D5" s="12">
+        <v>2</v>
+      </c>
+      <c r="E5" s="13">
+        <f>C5*D5</f>
+        <v>34.26</v>
+      </c>
+      <c r="F5" s="11">
+        <v>0</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="3">
+      <c r="B6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="3">
         <f>7.9 / 2</f>
         <v>3.95</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D6" s="17">
         <v>4</v>
       </c>
-      <c r="E4" s="3">
-        <f>C4*D4</f>
+      <c r="E6" s="3">
+        <f>C6*D6</f>
         <v>15.8</v>
       </c>
-      <c r="F4" s="11">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="F6" s="11">
+        <v>0</v>
+      </c>
+      <c r="G6" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I6" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="J4" s="14">
+      <c r="J6" s="14">
         <v>32850</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" s="3">
-        <v>3.2</v>
-      </c>
-      <c r="D5" s="1">
-        <v>2</v>
-      </c>
-      <c r="E5" s="3">
-        <f>C5*D5</f>
-        <v>6.4</v>
-      </c>
-      <c r="F5" s="11">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" t="s">
-        <v>38</v>
-      </c>
-      <c r="J5" s="14">
-        <v>32866</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="3">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="D6" s="1">
-        <v>2</v>
-      </c>
-      <c r="E6" s="16">
-        <f>C6*D6</f>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="F6" s="11">
-        <v>0</v>
-      </c>
-      <c r="I6" t="s">
-        <v>38</v>
-      </c>
-      <c r="J6" s="14">
-        <v>24760</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="1">
+        <v>59</v>
+      </c>
+      <c r="C7" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="D7" s="17">
         <v>2</v>
       </c>
+      <c r="E7" s="3">
+        <f>C7*D7</f>
+        <v>6.4</v>
+      </c>
       <c r="F7" s="11">
         <v>0</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H7" s="14">
-        <v>100056</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>41</v>
+      <c r="G7" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>38</v>
       </c>
       <c r="J7" s="14">
-        <v>100056</v>
+        <v>32866</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" s="1">
+        <v>59</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D8" s="17">
         <v>2</v>
       </c>
+      <c r="E8" s="16">
+        <f>C8*D8</f>
+        <v>2.2000000000000002</v>
+      </c>
       <c r="F8" s="11">
         <v>0</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" s="14">
+        <v>24760</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="17">
+        <v>2</v>
+      </c>
+      <c r="F9" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="11">
-        <v>0</v>
-      </c>
+      <c r="B10" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="17">
+        <v>6</v>
+      </c>
+      <c r="F14" s="11">
+        <v>0</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" s="14">
+        <v>100102</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="J14" s="14">
+        <v>100102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="30" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="27"/>
+      <c r="D15" s="32">
+        <f>4+2</f>
+        <v>6</v>
+      </c>
+      <c r="E15" s="27"/>
+      <c r="F15" s="28">
+        <v>0</v>
+      </c>
+      <c r="G15" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="H15" s="29">
+        <v>100089</v>
+      </c>
+      <c r="I15" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="J15" s="29">
+        <v>100089</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="17">
+        <v>2</v>
+      </c>
+      <c r="F16" s="11">
+        <v>0</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="H16" s="14">
+        <v>100056</v>
+      </c>
+      <c r="I16" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="J16" s="14">
+        <v>100056</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="30" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="25"/>
+      <c r="D17" s="27">
+        <f>2+8</f>
+        <v>10</v>
+      </c>
+      <c r="E17" s="25"/>
+      <c r="F17" s="28">
+        <v>0</v>
+      </c>
+      <c r="G17" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="H17" s="29">
+        <v>100315</v>
+      </c>
+      <c r="I17" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="J17" s="29">
+        <v>100315</v>
+      </c>
+      <c r="K17" s="25"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" xr:uid="{EF803173-6234-4D21-B2A0-29DFFED6055A}"/>
-    <hyperlink ref="K2" r:id="rId2" xr:uid="{1FD15487-DBA8-48D0-B21A-CD82C5F0DDA1}"/>
-    <hyperlink ref="J3" r:id="rId3" display="Lien" xr:uid="{590ADCCA-8CE7-40AA-8C96-4A2D1FC3681E}"/>
-    <hyperlink ref="J4" r:id="rId4" display="https://www.gotronic.fr/art-paire-de-moyeux-alu-1998-21781.htm" xr:uid="{244CC552-A9F4-455C-BE90-80AABB27A3FC}"/>
-    <hyperlink ref="J5" r:id="rId5" display="https://www.gotronic.fr/art-roue-libre-3-4-955-21789.htm" xr:uid="{9FA631D8-4924-422F-9436-0F4CC6AD4E31}"/>
-    <hyperlink ref="J6" r:id="rId6" location="complte_desc" display="https://www.gotronic.fr/art-roulement-19-6-6mm-157.htm - complte_desc" xr:uid="{668C1373-B577-40D7-AE22-CEC46B56C596}"/>
-    <hyperlink ref="H7" r:id="rId7" display="https://www.makerbeam.com/makerbeam-40mm-8p-black-makerbeam.html" xr:uid="{29B79743-9F8C-4F0D-B3CD-51472A8B11E8}"/>
-    <hyperlink ref="J7" r:id="rId8" display="https://www.makerbeam.com/makerbeam-40mm-8p-black-makerbeam.html" xr:uid="{82784541-8BB1-4123-8126-54CF8432B427}"/>
+    <hyperlink ref="J4" r:id="rId1" xr:uid="{EF803173-6234-4D21-B2A0-29DFFED6055A}"/>
+    <hyperlink ref="K4" r:id="rId2" xr:uid="{1FD15487-DBA8-48D0-B21A-CD82C5F0DDA1}"/>
+    <hyperlink ref="J5" r:id="rId3" display="Lien" xr:uid="{590ADCCA-8CE7-40AA-8C96-4A2D1FC3681E}"/>
+    <hyperlink ref="J6" r:id="rId4" display="https://www.gotronic.fr/art-paire-de-moyeux-alu-1998-21781.htm" xr:uid="{244CC552-A9F4-455C-BE90-80AABB27A3FC}"/>
+    <hyperlink ref="J7" r:id="rId5" display="https://www.gotronic.fr/art-roue-libre-3-4-955-21789.htm" xr:uid="{9FA631D8-4924-422F-9436-0F4CC6AD4E31}"/>
+    <hyperlink ref="J8" r:id="rId6" location="complte_desc" display="https://www.gotronic.fr/art-roulement-19-6-6mm-157.htm - complte_desc" xr:uid="{668C1373-B577-40D7-AE22-CEC46B56C596}"/>
+    <hyperlink ref="H16" r:id="rId7" display="https://www.makerbeam.com/makerbeam-40mm-8p-black-makerbeam.html" xr:uid="{29B79743-9F8C-4F0D-B3CD-51472A8B11E8}"/>
+    <hyperlink ref="J16" r:id="rId8" display="https://www.makerbeam.com/makerbeam-40mm-8p-black-makerbeam.html" xr:uid="{82784541-8BB1-4123-8126-54CF8432B427}"/>
+    <hyperlink ref="H17" r:id="rId9" display="https://www.makerbeam.com/makerbeam-corner-brackets-12p.html" xr:uid="{8FB5AF53-6074-4AC8-B954-48BA8EAD3BBD}"/>
+    <hyperlink ref="J17" r:id="rId10" display="https://www.makerbeam.com/makerbeam-corner-brackets-12p.html" xr:uid="{7056ADE0-0EF2-4579-9C02-59182784E373}"/>
+    <hyperlink ref="H14" r:id="rId11" display="https://www.makerbeam.com/makerbeam-300mm-4p-black-makerbeam.html" xr:uid="{820D934C-B464-4C2C-945E-E8BF995B725F}"/>
+    <hyperlink ref="J14" r:id="rId12" display="https://www.makerbeam.com/makerbeam-300mm-4p-black-makerbeam.html" xr:uid="{FA91347B-6F6D-4A03-9E56-95B5CEDF5974}"/>
+    <hyperlink ref="H15" r:id="rId13" display="https://www.makerbeam.com/makerbeam-150mm-6p-black-makerbeam.html" xr:uid="{FA27115A-E114-48C1-BFDF-2FC84C9726A7}"/>
+    <hyperlink ref="J15" r:id="rId14" display="https://www.makerbeam.com/makerbeam-150mm-6p-black-makerbeam.html" xr:uid="{6CDD4A5F-AA68-43CF-981B-AA5BC34F87A6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId9"/>
-  <legacyDrawing r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId15"/>
+  <legacyDrawing r:id="rId16"/>
 </worksheet>
 </file>
 
@@ -1057,7 +1260,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9B52879-989E-4911-9FCB-E5FD6170BF14}">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -1209,10 +1412,10 @@
       <c r="E5" s="11">
         <v>0</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="G5" s="17"/>
+      <c r="G5" s="18"/>
       <c r="H5" s="1" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
debut carte electronique base sur une Teensy
</commit_message>
<xml_diff>
--- a/Mecanique/BOM Mecanique.xlsx
+++ b/Mecanique/BOM Mecanique.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git folder\my_robot\Mecanique\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B76E5CB-4A89-49FA-9AA8-8F58C851114A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37904FB2-4B99-467E-94AA-34A9F6FA8F41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Articles achetés" sheetId="1" r:id="rId1"/>
-    <sheet name="Articles fabriqués" sheetId="2" r:id="rId2"/>
+    <sheet name="Elements achetes" sheetId="1" r:id="rId1"/>
+    <sheet name="Elements fabriques" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -134,7 +134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="61">
   <si>
     <t>Mecanique/Base roulante</t>
   </si>
@@ -310,24 +310,14 @@
     <t>Profilé MakerBeam 150mm</t>
   </si>
   <si>
-    <t>Groupe(s)</t>
-  </si>
-  <si>
     <t>Base roulante</t>
   </si>
   <si>
-    <t>Structure</t>
-  </si>
-  <si>
-    <t>Base roulante
-Structure</t>
-  </si>
-  <si>
     <t>Pneu (à partir d'une chambre à air de vélo)</t>
   </si>
   <si>
-    <t>Structure
-Etage actionneurs</t>
+    <t>Quantité
+total</t>
   </si>
 </sst>
 </file>
@@ -424,7 +414,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -477,9 +467,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -500,9 +487,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -515,10 +499,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -844,411 +828,368 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="55.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="17" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" style="17" customWidth="1"/>
-    <col min="8" max="8" width="21.85546875" style="15" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" style="17" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" style="15" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="17" customWidth="1"/>
+    <col min="3" max="4" width="10.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" style="17" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" style="15" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" style="17" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" style="15" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>58</v>
+      <c r="B1" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>19</v>
       </c>
+      <c r="F1" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="G1" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="21" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-    </row>
-    <row r="3" spans="1:11" s="23" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="18"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+    </row>
+    <row r="3" spans="1:10" s="22" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="19"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>59</v>
+      <c r="B4" s="17">
+        <v>2</v>
       </c>
       <c r="C4" s="3">
         <v>20.9</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="3">
+        <f>C4*B4</f>
+        <v>41.8</v>
+      </c>
+      <c r="E4" s="9">
         <v>2</v>
       </c>
-      <c r="E4" s="3">
-        <f>C4*D4</f>
-        <v>41.8</v>
-      </c>
-      <c r="F4" s="9">
-        <v>2</v>
-      </c>
-      <c r="G4" s="17" t="s">
+      <c r="F4" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="17" t="s">
+      <c r="H4" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="I4" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="J4" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
-      <c r="B5" t="s">
-        <v>59</v>
+      <c r="B5" s="12">
+        <v>2</v>
       </c>
       <c r="C5" s="3">
         <v>17.13</v>
       </c>
-      <c r="D5" s="12">
-        <v>2</v>
-      </c>
-      <c r="E5" s="13">
-        <f>C5*D5</f>
+      <c r="D5" s="13">
+        <f>C5*B5</f>
         <v>34.26</v>
       </c>
-      <c r="F5" s="11">
-        <v>0</v>
-      </c>
-      <c r="H5" s="15" t="s">
+      <c r="E5" s="11">
+        <v>0</v>
+      </c>
+      <c r="G5" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="I5" s="17" t="s">
+      <c r="H5" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="14" t="s">
+      <c r="I5" s="14" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>37</v>
       </c>
-      <c r="B6" t="s">
-        <v>59</v>
+      <c r="B6" s="17">
+        <v>4</v>
       </c>
       <c r="C6" s="3">
         <f>7.9 / 2</f>
         <v>3.95</v>
       </c>
-      <c r="D6" s="17">
-        <v>4</v>
-      </c>
-      <c r="E6" s="3">
-        <f>C6*D6</f>
+      <c r="D6" s="3">
+        <f>C6*B6</f>
         <v>15.8</v>
       </c>
-      <c r="F6" s="11">
-        <v>0</v>
-      </c>
-      <c r="G6" s="17" t="s">
+      <c r="E6" s="11">
+        <v>0</v>
+      </c>
+      <c r="F6" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="H6" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="J6" s="14">
+      <c r="I6" s="14">
         <v>32850</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>53</v>
       </c>
-      <c r="B7" t="s">
-        <v>59</v>
+      <c r="B7" s="17">
+        <v>2</v>
       </c>
       <c r="C7" s="3">
         <v>3.2</v>
       </c>
-      <c r="D7" s="17">
-        <v>2</v>
-      </c>
-      <c r="E7" s="3">
-        <f>C7*D7</f>
+      <c r="D7" s="3">
+        <f>C7*B7</f>
         <v>6.4</v>
       </c>
-      <c r="F7" s="11">
-        <v>0</v>
-      </c>
-      <c r="G7" s="17" t="s">
+      <c r="E7" s="11">
+        <v>0</v>
+      </c>
+      <c r="F7" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="17" t="s">
+      <c r="H7" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="J7" s="14">
+      <c r="I7" s="14">
         <v>32866</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>39</v>
       </c>
-      <c r="B8" t="s">
-        <v>59</v>
+      <c r="B8" s="17">
+        <v>2</v>
       </c>
       <c r="C8" s="3">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D8" s="17">
-        <v>2</v>
-      </c>
-      <c r="E8" s="16">
-        <f>C8*D8</f>
+      <c r="D8" s="16">
+        <f>C8*B8</f>
         <v>2.2000000000000002</v>
       </c>
-      <c r="F8" s="11">
-        <v>0</v>
-      </c>
-      <c r="I8" s="17" t="s">
+      <c r="E8" s="11">
+        <v>0</v>
+      </c>
+      <c r="H8" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="14">
+      <c r="I8" s="14">
         <v>24760</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>42</v>
       </c>
-      <c r="B9" t="s">
-        <v>59</v>
-      </c>
-      <c r="D9" s="17">
+      <c r="B9" s="17">
         <v>2</v>
       </c>
-      <c r="F9" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E9" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>51</v>
       </c>
-      <c r="B10" t="s">
+      <c r="E10" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>59</v>
       </c>
-      <c r="F10" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" t="s">
-        <v>59</v>
-      </c>
       <c r="C11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
+      <c r="D11" s="17"/>
+      <c r="E11" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="23" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>56</v>
       </c>
-      <c r="B14" t="s">
-        <v>60</v>
-      </c>
-      <c r="D14" s="17">
+      <c r="B14" s="17">
         <v>6</v>
       </c>
-      <c r="F14" s="11">
-        <v>0</v>
-      </c>
-      <c r="G14" s="17" t="s">
+      <c r="E14" s="11">
+        <v>0</v>
+      </c>
+      <c r="F14" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="H14" s="14">
+      <c r="G14" s="14">
         <v>100102</v>
       </c>
-      <c r="I14" s="17" t="s">
+      <c r="H14" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="J14" s="14">
+      <c r="I14" s="14">
         <v>100102</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="30" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="30" t="s">
+    <row r="15" spans="1:10" s="28" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="B15" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="C15" s="27"/>
-      <c r="D15" s="32">
+      <c r="B15" s="29">
         <f>4+2</f>
         <v>6</v>
       </c>
-      <c r="E15" s="27"/>
-      <c r="F15" s="28">
-        <v>0</v>
-      </c>
-      <c r="G15" s="27" t="s">
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="26">
+        <v>0</v>
+      </c>
+      <c r="F15" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="H15" s="29">
+      <c r="G15" s="27">
         <v>100089</v>
       </c>
-      <c r="I15" s="27" t="s">
+      <c r="H15" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="J15" s="29">
+      <c r="I15" s="27">
         <v>100089</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>40</v>
       </c>
-      <c r="B16" t="s">
-        <v>59</v>
-      </c>
-      <c r="D16" s="17">
+      <c r="B16" s="17">
         <v>2</v>
       </c>
-      <c r="F16" s="11">
-        <v>0</v>
-      </c>
-      <c r="G16" s="17" t="s">
+      <c r="E16" s="11">
+        <v>0</v>
+      </c>
+      <c r="F16" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="H16" s="14">
+      <c r="G16" s="14">
         <v>100056</v>
       </c>
-      <c r="I16" s="17" t="s">
+      <c r="H16" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="J16" s="14">
+      <c r="I16" s="14">
         <v>100056</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="30" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
+    <row r="17" spans="1:10" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="25"/>
-      <c r="D17" s="27">
+      <c r="B17" s="25">
         <f>2+8</f>
         <v>10</v>
       </c>
-      <c r="E17" s="25"/>
-      <c r="F17" s="28">
-        <v>0</v>
-      </c>
-      <c r="G17" s="27" t="s">
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="26">
+        <v>0</v>
+      </c>
+      <c r="F17" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="H17" s="29">
+      <c r="G17" s="27">
         <v>100315</v>
       </c>
-      <c r="I17" s="27" t="s">
+      <c r="H17" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="J17" s="29">
+      <c r="I17" s="27">
         <v>100315</v>
       </c>
-      <c r="K17" s="25"/>
+      <c r="J17" s="24"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J4" r:id="rId1" xr:uid="{EF803173-6234-4D21-B2A0-29DFFED6055A}"/>
-    <hyperlink ref="K4" r:id="rId2" xr:uid="{1FD15487-DBA8-48D0-B21A-CD82C5F0DDA1}"/>
-    <hyperlink ref="J5" r:id="rId3" display="Lien" xr:uid="{590ADCCA-8CE7-40AA-8C96-4A2D1FC3681E}"/>
-    <hyperlink ref="J6" r:id="rId4" display="https://www.gotronic.fr/art-paire-de-moyeux-alu-1998-21781.htm" xr:uid="{244CC552-A9F4-455C-BE90-80AABB27A3FC}"/>
-    <hyperlink ref="J7" r:id="rId5" display="https://www.gotronic.fr/art-roue-libre-3-4-955-21789.htm" xr:uid="{9FA631D8-4924-422F-9436-0F4CC6AD4E31}"/>
-    <hyperlink ref="J8" r:id="rId6" location="complte_desc" display="https://www.gotronic.fr/art-roulement-19-6-6mm-157.htm - complte_desc" xr:uid="{668C1373-B577-40D7-AE22-CEC46B56C596}"/>
-    <hyperlink ref="H16" r:id="rId7" display="https://www.makerbeam.com/makerbeam-40mm-8p-black-makerbeam.html" xr:uid="{29B79743-9F8C-4F0D-B3CD-51472A8B11E8}"/>
-    <hyperlink ref="J16" r:id="rId8" display="https://www.makerbeam.com/makerbeam-40mm-8p-black-makerbeam.html" xr:uid="{82784541-8BB1-4123-8126-54CF8432B427}"/>
-    <hyperlink ref="H17" r:id="rId9" display="https://www.makerbeam.com/makerbeam-corner-brackets-12p.html" xr:uid="{8FB5AF53-6074-4AC8-B954-48BA8EAD3BBD}"/>
-    <hyperlink ref="J17" r:id="rId10" display="https://www.makerbeam.com/makerbeam-corner-brackets-12p.html" xr:uid="{7056ADE0-0EF2-4579-9C02-59182784E373}"/>
-    <hyperlink ref="H14" r:id="rId11" display="https://www.makerbeam.com/makerbeam-300mm-4p-black-makerbeam.html" xr:uid="{820D934C-B464-4C2C-945E-E8BF995B725F}"/>
-    <hyperlink ref="J14" r:id="rId12" display="https://www.makerbeam.com/makerbeam-300mm-4p-black-makerbeam.html" xr:uid="{FA91347B-6F6D-4A03-9E56-95B5CEDF5974}"/>
-    <hyperlink ref="H15" r:id="rId13" display="https://www.makerbeam.com/makerbeam-150mm-6p-black-makerbeam.html" xr:uid="{FA27115A-E114-48C1-BFDF-2FC84C9726A7}"/>
-    <hyperlink ref="J15" r:id="rId14" display="https://www.makerbeam.com/makerbeam-150mm-6p-black-makerbeam.html" xr:uid="{6CDD4A5F-AA68-43CF-981B-AA5BC34F87A6}"/>
+    <hyperlink ref="I4" r:id="rId1" xr:uid="{EF803173-6234-4D21-B2A0-29DFFED6055A}"/>
+    <hyperlink ref="J4" r:id="rId2" xr:uid="{1FD15487-DBA8-48D0-B21A-CD82C5F0DDA1}"/>
+    <hyperlink ref="I5" r:id="rId3" display="Lien" xr:uid="{590ADCCA-8CE7-40AA-8C96-4A2D1FC3681E}"/>
+    <hyperlink ref="I6" r:id="rId4" display="https://www.gotronic.fr/art-paire-de-moyeux-alu-1998-21781.htm" xr:uid="{244CC552-A9F4-455C-BE90-80AABB27A3FC}"/>
+    <hyperlink ref="I7" r:id="rId5" display="https://www.gotronic.fr/art-roue-libre-3-4-955-21789.htm" xr:uid="{9FA631D8-4924-422F-9436-0F4CC6AD4E31}"/>
+    <hyperlink ref="I8" r:id="rId6" location="complte_desc" display="https://www.gotronic.fr/art-roulement-19-6-6mm-157.htm - complte_desc" xr:uid="{668C1373-B577-40D7-AE22-CEC46B56C596}"/>
+    <hyperlink ref="G16" r:id="rId7" display="https://www.makerbeam.com/makerbeam-40mm-8p-black-makerbeam.html" xr:uid="{29B79743-9F8C-4F0D-B3CD-51472A8B11E8}"/>
+    <hyperlink ref="I16" r:id="rId8" display="https://www.makerbeam.com/makerbeam-40mm-8p-black-makerbeam.html" xr:uid="{82784541-8BB1-4123-8126-54CF8432B427}"/>
+    <hyperlink ref="G17" r:id="rId9" display="https://www.makerbeam.com/makerbeam-corner-brackets-12p.html" xr:uid="{8FB5AF53-6074-4AC8-B954-48BA8EAD3BBD}"/>
+    <hyperlink ref="I17" r:id="rId10" display="https://www.makerbeam.com/makerbeam-corner-brackets-12p.html" xr:uid="{7056ADE0-0EF2-4579-9C02-59182784E373}"/>
+    <hyperlink ref="G14" r:id="rId11" display="https://www.makerbeam.com/makerbeam-300mm-4p-black-makerbeam.html" xr:uid="{820D934C-B464-4C2C-945E-E8BF995B725F}"/>
+    <hyperlink ref="I14" r:id="rId12" display="https://www.makerbeam.com/makerbeam-300mm-4p-black-makerbeam.html" xr:uid="{FA91347B-6F6D-4A03-9E56-95B5CEDF5974}"/>
+    <hyperlink ref="G15" r:id="rId13" display="https://www.makerbeam.com/makerbeam-150mm-6p-black-makerbeam.html" xr:uid="{FA27115A-E114-48C1-BFDF-2FC84C9726A7}"/>
+    <hyperlink ref="I15" r:id="rId14" display="https://www.makerbeam.com/makerbeam-150mm-6p-black-makerbeam.html" xr:uid="{6CDD4A5F-AA68-43CF-981B-AA5BC34F87A6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId15"/>
@@ -1261,7 +1202,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1412,10 +1353,10 @@
       <c r="E5" s="11">
         <v>0</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="G5" s="18"/>
+      <c r="G5" s="30"/>
       <c r="H5" s="1" t="s">
         <v>45</v>
       </c>

</xml_diff>